<commit_message>
Colisoes com terreno e com combustivel OK, falta os avioes com bezier
</commit_message>
<xml_diff>
--- a/TexturaAsfalto/Mapas.xlsx
+++ b/TexturaAsfalto/Mapas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marciopinho/Dropbox/CG/OpenGL/Testes/SimuladorDeCidade/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Trabalhos\20211\CG\FCG_T3\TexturaAsfalto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F09918C-E683-114D-9934-D1D5AEC820CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EE13F8-BF8B-43B6-9F06-3642C003EF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="27420" windowHeight="16900" xr2:uid="{FC2CF6D7-3F9B-634F-990F-D08FA91C538E}"/>
+    <workbookView xWindow="15255" yWindow="1005" windowWidth="17355" windowHeight="14850" xr2:uid="{FC2CF6D7-3F9B-634F-990F-D08FA91C538E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +118,13 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -152,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -173,6 +180,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,20 +497,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1046F0D-B5FA-8D4B-B55C-04017372D161}">
   <dimension ref="A2:BB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="8.625" customWidth="1"/>
+    <col min="3" max="3" width="11.375" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="50" width="2.83203125" customWidth="1"/>
+    <col min="5" max="50" width="2.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54">
       <c r="E2" s="4">
         <v>0</v>
       </c>
@@ -654,7 +662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -801,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54">
       <c r="B4" s="3"/>
       <c r="D4" s="4">
         <v>1</v>
@@ -945,7 +953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1547,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1697,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1847,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -1997,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -2147,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2297,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -2447,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
@@ -2597,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -2747,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -2896,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -3045,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50">
       <c r="D19" s="4">
         <v>16</v>
       </c>
@@ -3188,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50">
       <c r="D20" s="4">
         <v>17</v>
       </c>
@@ -3331,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50">
       <c r="D21" s="4">
         <v>18</v>
       </c>
@@ -3474,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50">
       <c r="D22" s="4">
         <v>19</v>
       </c>
@@ -3617,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50">
       <c r="D23" s="4">
         <v>20</v>
       </c>
@@ -3760,7 +3768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50">
       <c r="D24" s="4">
         <v>21</v>
       </c>
@@ -3903,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:50">
       <c r="D25" s="4">
         <v>22</v>
       </c>
@@ -4046,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50">
       <c r="D26" s="4">
         <v>23</v>
       </c>
@@ -4189,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50">
       <c r="D27" s="4">
         <v>24</v>
       </c>
@@ -4332,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50">
       <c r="D28" s="4">
         <v>25</v>
       </c>
@@ -4475,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50">
       <c r="D29" s="4">
         <v>26</v>
       </c>
@@ -4618,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50">
       <c r="D30" s="4">
         <v>27</v>
       </c>
@@ -4761,7 +4769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50">
       <c r="D31" s="4">
         <v>28</v>
       </c>
@@ -4904,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50">
       <c r="D32" s="4">
         <v>29</v>
       </c>
@@ -5047,45 +5055,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:50">
       <c r="D33" s="4">
         <v>30</v>
       </c>
       <c r="E33" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J33" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K33" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O33" s="2">
-        <v>0</v>
-      </c>
-      <c r="P33" s="2">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="P33" s="10">
+        <v>4</v>
       </c>
       <c r="Q33" s="2">
         <v>0</v>
@@ -5190,45 +5198,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:50">
       <c r="D34" s="4">
         <v>31</v>
       </c>
       <c r="E34" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J34" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K34" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P34" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q34" s="2">
         <v>0</v>
@@ -5333,45 +5341,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:50">
       <c r="D35" s="4">
         <v>32</v>
       </c>
       <c r="E35" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F35" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G35" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H35" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I35" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J35" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K35" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L35" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M35" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N35" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O35" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P35" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q35" s="2">
         <v>0</v>
@@ -5476,45 +5484,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:50">
       <c r="D36" s="4">
         <v>33</v>
       </c>
       <c r="E36" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J36" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K36" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N36" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O36" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P36" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q36" s="2">
         <v>0</v>
@@ -5619,45 +5627,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:50">
       <c r="D37" s="4">
         <v>34</v>
       </c>
       <c r="E37" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N37" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O37" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P37" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q37" s="2">
         <v>0</v>
@@ -5762,45 +5770,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:50">
       <c r="D38" s="4">
         <v>35</v>
       </c>
       <c r="E38" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J38" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K38" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P38" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q38" s="2">
         <v>0</v>
@@ -5905,45 +5913,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:50">
       <c r="D39" s="4">
         <v>36</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I39" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J39" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K39" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L39" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M39" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N39" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O39" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P39" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q39" s="2">
         <v>0</v>
@@ -6048,45 +6056,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:50">
       <c r="D40" s="4">
         <v>37</v>
       </c>
       <c r="E40" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G40" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J40" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K40" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P40" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q40" s="2">
         <v>0</v>
@@ -6191,45 +6199,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:50">
       <c r="D41" s="4">
         <v>38</v>
       </c>
       <c r="E41" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F41" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H41" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I41" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M41" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N41" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O41" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P41" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q41" s="2">
         <v>0</v>
@@ -6334,45 +6342,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:50">
       <c r="D42" s="4">
         <v>39</v>
       </c>
       <c r="E42" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F42" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G42" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H42" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I42" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J42" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K42" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L42" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M42" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N42" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O42" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P42" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q42" s="2">
         <v>0</v>
@@ -6477,45 +6485,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:50">
       <c r="D43" s="4">
         <v>40</v>
       </c>
       <c r="E43" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O43" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P43" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q43" s="2">
         <v>0</v>
@@ -6620,45 +6628,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:50">
       <c r="D44" s="4">
         <v>41</v>
       </c>
       <c r="E44" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O44" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P44" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q44" s="2">
         <v>0</v>
@@ -6763,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:50">
       <c r="D45" s="4">
         <v>42</v>
       </c>
@@ -6906,7 +6914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:50">
       <c r="D46" s="4">
         <v>43</v>
       </c>
@@ -7049,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:50">
       <c r="D47" s="4">
         <v>44</v>
       </c>
@@ -7192,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:50">
       <c r="D48" s="4">
         <v>45</v>
       </c>
@@ -7335,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:50">
       <c r="D49" s="4">
         <v>46</v>
       </c>
@@ -7478,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:50">
       <c r="D50" s="4">
         <v>47</v>
       </c>
@@ -7621,7 +7629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:50">
       <c r="D51" s="4">
         <v>48</v>
       </c>
@@ -7764,7 +7772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:50" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:50">
       <c r="D52" s="4">
         <v>49</v>
       </c>
@@ -7909,5 +7917,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
N aguento mais essa porra
</commit_message>
<xml_diff>
--- a/TexturaAsfalto/Mapas.xlsx
+++ b/TexturaAsfalto/Mapas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Trabalhos\20211\CG\FCG_T3\TexturaAsfalto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EE13F8-BF8B-43B6-9F06-3642C003EF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4DF81E-D41D-4202-B937-9501781D2B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15255" yWindow="1005" windowWidth="17355" windowHeight="14850" xr2:uid="{FC2CF6D7-3F9B-634F-990F-D08FA91C538E}"/>
+    <workbookView xWindow="12630" yWindow="2910" windowWidth="25035" windowHeight="14850" xr2:uid="{FC2CF6D7-3F9B-634F-990F-D08FA91C538E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +122,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -181,6 +189,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1046F0D-B5FA-8D4B-B55C-04017372D161}">
   <dimension ref="A2:BB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="P44" sqref="E33:P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -815,13 +824,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
         <v>4</v>
       </c>
-      <c r="F4" s="9">
-        <v>5</v>
-      </c>
       <c r="G4" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H4" s="9">
         <v>5</v>
@@ -896,13 +905,13 @@
         <v>5</v>
       </c>
       <c r="AF4" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AG4" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AH4" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="2">
         <v>5</v>
@@ -967,91 +976,91 @@
         <v>2</v>
       </c>
       <c r="E5" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F5" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S5" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="T5" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="9">
         <v>7</v>
       </c>
       <c r="AB5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE5" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH5" s="9">
         <v>0</v>
@@ -1117,13 +1126,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H6" s="9">
         <v>0</v>
@@ -1198,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="AF6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG6" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH6" s="9">
         <v>0</v>
@@ -1267,13 +1276,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7" s="9">
         <v>0</v>
@@ -1348,10 +1357,10 @@
         <v>0</v>
       </c>
       <c r="AF7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH7" s="9">
         <v>0</v>
@@ -1417,28 +1426,28 @@
         <v>5</v>
       </c>
       <c r="E8" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F8" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G8" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H8" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J8" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L8" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="9">
         <v>0</v>
@@ -1498,10 +1507,10 @@
         <v>0</v>
       </c>
       <c r="AF8" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG8" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH8" s="9">
         <v>0</v>
@@ -1567,13 +1576,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F9" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G9" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H9" s="9">
         <v>0</v>
@@ -1588,28 +1597,28 @@
         <v>0</v>
       </c>
       <c r="L9" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M9" s="9">
         <v>0</v>
       </c>
       <c r="N9" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O9" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P9" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R9" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S9" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="T9" s="9">
         <v>7</v>
@@ -1648,10 +1657,10 @@
         <v>0</v>
       </c>
       <c r="AF9" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG9" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH9" s="9">
         <v>0</v>
@@ -1717,13 +1726,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F10" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G10" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H10" s="9">
         <v>0</v>
@@ -1738,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M10" s="9">
         <v>0</v>
@@ -1750,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q10" s="9">
         <v>0</v>
@@ -1798,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="AF10" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG10" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH10" s="9">
         <v>0</v>
@@ -1867,13 +1876,13 @@
         <v>8</v>
       </c>
       <c r="E11" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F11" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G11" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H11" s="9">
         <v>0</v>
@@ -1888,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M11" s="9">
         <v>0</v>
@@ -1900,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q11" s="9">
         <v>0</v>
@@ -1921,7 +1930,7 @@
         <v>0</v>
       </c>
       <c r="W11" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X11" s="9">
         <v>5</v>
@@ -1948,10 +1957,10 @@
         <v>0</v>
       </c>
       <c r="AF11" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG11" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH11" s="9">
         <v>0</v>
@@ -2017,13 +2026,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H12" s="9">
         <v>0</v>
@@ -2038,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M12" s="9">
         <v>0</v>
@@ -2050,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q12" s="9">
         <v>0</v>
@@ -2098,10 +2107,10 @@
         <v>0</v>
       </c>
       <c r="AF12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG12" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH12" s="9">
         <v>0</v>
@@ -2167,13 +2176,13 @@
         <v>10</v>
       </c>
       <c r="E13" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H13" s="9">
         <v>0</v>
@@ -2188,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M13" s="9">
         <v>0</v>
@@ -2200,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="9">
         <v>0</v>
@@ -2248,10 +2257,10 @@
         <v>0</v>
       </c>
       <c r="AF13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG13" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH13" s="9">
         <v>0</v>
@@ -2317,13 +2326,13 @@
         <v>11</v>
       </c>
       <c r="E14" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F14" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G14" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H14" s="9">
         <v>0</v>
@@ -2338,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M14" s="9">
         <v>0</v>
@@ -2350,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q14" s="9">
         <v>0</v>
@@ -2398,10 +2407,10 @@
         <v>0</v>
       </c>
       <c r="AF14" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG14" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH14" s="9">
         <v>0</v>
@@ -2467,13 +2476,13 @@
         <v>12</v>
       </c>
       <c r="E15" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H15" s="9">
         <v>0</v>
@@ -2488,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M15" s="9">
         <v>0</v>
@@ -2500,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q15" s="9">
         <v>0</v>
@@ -2548,10 +2557,10 @@
         <v>0</v>
       </c>
       <c r="AF15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH15" s="9">
         <v>0</v>
@@ -2617,13 +2626,13 @@
         <v>13</v>
       </c>
       <c r="E16" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F16" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G16" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H16" s="9">
         <v>0</v>
@@ -2638,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M16" s="9">
         <v>0</v>
@@ -2650,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q16" s="9">
         <v>0</v>
@@ -2698,10 +2707,10 @@
         <v>0</v>
       </c>
       <c r="AF16" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG16" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH16" s="9">
         <v>0</v>
@@ -2766,40 +2775,40 @@
         <v>14</v>
       </c>
       <c r="E17" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F17" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G17" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P17" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="9">
         <v>0</v>
@@ -2847,10 +2856,10 @@
         <v>0</v>
       </c>
       <c r="AF17" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG17" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH17" s="9">
         <v>0</v>
@@ -2915,13 +2924,13 @@
         <v>15</v>
       </c>
       <c r="E18" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F18" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G18" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H18" s="9">
         <v>0</v>
@@ -2936,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M18" s="9">
         <v>0</v>
@@ -2996,10 +3005,10 @@
         <v>0</v>
       </c>
       <c r="AF18" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG18" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH18" s="9">
         <v>0</v>
@@ -3058,13 +3067,13 @@
         <v>16</v>
       </c>
       <c r="E19" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F19" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G19" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H19" s="9">
         <v>0</v>
@@ -3079,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M19" s="9">
         <v>0</v>
@@ -3139,10 +3148,10 @@
         <v>0</v>
       </c>
       <c r="AF19" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG19" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH19" s="9">
         <v>0</v>
@@ -3201,13 +3210,13 @@
         <v>17</v>
       </c>
       <c r="E20" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F20" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G20" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H20" s="9">
         <v>0</v>
@@ -3222,16 +3231,16 @@
         <v>0</v>
       </c>
       <c r="L20" s="9">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M20" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N20" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O20" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P20" s="9">
         <v>0</v>
@@ -3282,10 +3291,10 @@
         <v>0</v>
       </c>
       <c r="AF20" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG20" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH20" s="9">
         <v>0</v>
@@ -3344,13 +3353,13 @@
         <v>18</v>
       </c>
       <c r="E21" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F21" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G21" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H21" s="9">
         <v>0</v>
@@ -3425,10 +3434,10 @@
         <v>0</v>
       </c>
       <c r="AF21" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG21" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH21" s="9">
         <v>0</v>
@@ -3487,13 +3496,13 @@
         <v>19</v>
       </c>
       <c r="E22" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F22" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G22" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H22" s="9">
         <v>0</v>
@@ -3568,10 +3577,10 @@
         <v>0</v>
       </c>
       <c r="AF22" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG22" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH22" s="9">
         <v>0</v>
@@ -3630,13 +3639,13 @@
         <v>20</v>
       </c>
       <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
         <v>9</v>
       </c>
-      <c r="F23" s="9">
-        <v>5</v>
-      </c>
       <c r="G23" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H23" s="9">
         <v>5</v>
@@ -3711,13 +3720,13 @@
         <v>5</v>
       </c>
       <c r="AF23" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AG23" s="9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AH23" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI23" s="2">
         <v>5</v>
@@ -3773,91 +3782,91 @@
         <v>21</v>
       </c>
       <c r="E24" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F24" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S24" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="T24" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA24" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE24" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG24" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH24" s="9">
         <v>0</v>
@@ -3916,13 +3925,13 @@
         <v>22</v>
       </c>
       <c r="E25" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F25" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G25" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H25" s="9">
         <v>0</v>
@@ -3931,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K25" s="9">
         <v>0</v>
@@ -3949,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q25" s="9">
         <v>0</v>
@@ -3997,10 +4006,10 @@
         <v>0</v>
       </c>
       <c r="AF25" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG25" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH25" s="9">
         <v>0</v>
@@ -4059,13 +4068,13 @@
         <v>23</v>
       </c>
       <c r="E26" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F26" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G26" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H26" s="9">
         <v>0</v>
@@ -4074,7 +4083,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K26" s="9">
         <v>0</v>
@@ -4092,7 +4101,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q26" s="9">
         <v>0</v>
@@ -4140,10 +4149,10 @@
         <v>0</v>
       </c>
       <c r="AF26" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG26" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH26" s="9">
         <v>0</v>
@@ -4202,13 +4211,13 @@
         <v>24</v>
       </c>
       <c r="E27" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F27" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G27" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H27" s="9">
         <v>0</v>
@@ -4217,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K27" s="9">
         <v>0</v>
@@ -4235,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q27" s="9">
         <v>0</v>
@@ -4283,10 +4292,10 @@
         <v>0</v>
       </c>
       <c r="AF27" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG27" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH27" s="9">
         <v>0</v>
@@ -4345,13 +4354,13 @@
         <v>25</v>
       </c>
       <c r="E28" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F28" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G28" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H28" s="9">
         <v>0</v>
@@ -4378,7 +4387,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q28" s="9">
         <v>0</v>
@@ -4426,10 +4435,10 @@
         <v>0</v>
       </c>
       <c r="AF28" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG28" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AH28" s="9">
         <v>0</v>
@@ -4488,13 +4497,13 @@
         <v>26</v>
       </c>
       <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
         <v>9</v>
       </c>
-      <c r="F29" s="9">
-        <v>5</v>
-      </c>
       <c r="G29" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H29" s="9">
         <v>5</v>
@@ -4521,7 +4530,7 @@
         <v>5</v>
       </c>
       <c r="P29" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="9">
         <v>5</v>
@@ -4569,13 +4578,13 @@
         <v>5</v>
       </c>
       <c r="AF29" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AG29" s="9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AH29" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI29" s="2">
         <v>0</v>
@@ -4631,91 +4640,91 @@
         <v>27</v>
       </c>
       <c r="E30" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F30" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S30" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="T30" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA30" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AB30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE30" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG30" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH30" s="9">
         <v>0</v>
@@ -4774,91 +4783,91 @@
         <v>28</v>
       </c>
       <c r="E31" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F31" s="9">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G31" s="9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S31" s="9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="T31" s="9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="U31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA31" s="9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AB31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE31" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF31" s="9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AG31" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AH31" s="9">
         <v>0</v>
@@ -4917,94 +4926,94 @@
         <v>29</v>
       </c>
       <c r="E32" s="9">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S32" s="9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="T32" s="9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="U32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Z32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AA32" s="9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AB32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AC32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AD32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AE32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AF32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AG32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AH32" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI32" s="2">
         <v>0</v>
@@ -5055,12 +5064,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:50">
+    <row r="33" spans="3:50">
       <c r="D33" s="4">
         <v>30</v>
       </c>
       <c r="E33" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F33" s="2">
         <v>5</v>
@@ -5093,7 +5102,7 @@
         <v>5</v>
       </c>
       <c r="P33" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q33" s="2">
         <v>0</v>
@@ -5198,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:50">
+    <row r="34" spans="3:50">
       <c r="D34" s="4">
         <v>31</v>
       </c>
@@ -5218,10 +5227,10 @@
         <v>6</v>
       </c>
       <c r="J34" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K34" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L34" s="2">
         <v>6</v>
@@ -5341,7 +5350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:50">
+    <row r="35" spans="3:50">
       <c r="D35" s="4">
         <v>32</v>
       </c>
@@ -5361,10 +5370,10 @@
         <v>6</v>
       </c>
       <c r="J35" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K35" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L35" s="2">
         <v>6</v>
@@ -5484,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:50">
+    <row r="36" spans="3:50">
       <c r="D36" s="4">
         <v>33</v>
       </c>
@@ -5504,10 +5513,10 @@
         <v>6</v>
       </c>
       <c r="J36" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K36" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L36" s="2">
         <v>6</v>
@@ -5516,7 +5525,7 @@
         <v>6</v>
       </c>
       <c r="N36" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O36" s="2">
         <v>6</v>
@@ -5627,7 +5636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:50">
+    <row r="37" spans="3:50">
       <c r="D37" s="4">
         <v>34</v>
       </c>
@@ -5770,7 +5779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:50">
+    <row r="38" spans="3:50">
       <c r="D38" s="4">
         <v>35</v>
       </c>
@@ -5790,10 +5799,10 @@
         <v>6</v>
       </c>
       <c r="J38" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K38" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L38" s="2">
         <v>6</v>
@@ -5913,7 +5922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:50">
+    <row r="39" spans="3:50">
       <c r="D39" s="4">
         <v>36</v>
       </c>
@@ -5933,10 +5942,10 @@
         <v>6</v>
       </c>
       <c r="J39" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K39" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L39" s="2">
         <v>6</v>
@@ -6056,7 +6065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:50">
+    <row r="40" spans="3:50">
       <c r="D40" s="4">
         <v>37</v>
       </c>
@@ -6076,10 +6085,10 @@
         <v>6</v>
       </c>
       <c r="J40" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K40" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L40" s="2">
         <v>6</v>
@@ -6199,7 +6208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:50">
+    <row r="41" spans="3:50">
       <c r="D41" s="4">
         <v>38</v>
       </c>
@@ -6216,7 +6225,7 @@
         <v>12</v>
       </c>
       <c r="I41" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J41" s="2">
         <v>1</v>
@@ -6342,7 +6351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:50">
+    <row r="42" spans="3:50">
       <c r="D42" s="4">
         <v>39</v>
       </c>
@@ -6362,10 +6371,10 @@
         <v>6</v>
       </c>
       <c r="J42" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K42" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="L42" s="2">
         <v>5</v>
@@ -6485,7 +6494,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:50">
+    <row r="43" spans="3:50">
+      <c r="C43" s="11"/>
       <c r="D43" s="4">
         <v>40</v>
       </c>
@@ -6628,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:50">
+    <row r="44" spans="3:50">
       <c r="D44" s="4">
         <v>41</v>
       </c>
@@ -6771,7 +6781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:50">
+    <row r="45" spans="3:50">
       <c r="D45" s="4">
         <v>42</v>
       </c>
@@ -6914,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:50">
+    <row r="46" spans="3:50">
       <c r="D46" s="4">
         <v>43</v>
       </c>
@@ -7057,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:50">
+    <row r="47" spans="3:50">
       <c r="D47" s="4">
         <v>44</v>
       </c>
@@ -7200,7 +7210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:50">
+    <row r="48" spans="3:50">
       <c r="D48" s="4">
         <v>45</v>
       </c>

</xml_diff>